<commit_message>
alomst made it work
</commit_message>
<xml_diff>
--- a/New Grades.xlsx
+++ b/New Grades.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1:XFD1048576"/>
@@ -492,6 +492,216 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>1</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>John</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Joey</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Greg</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Arielie</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Lisa</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Bob</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>2</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>John</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Joey</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Greg</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Arielie</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Lisa</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Bob</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>3</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>John</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Joey</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Greg</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Arielie</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Lisa</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Bob</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>4</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>John</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Joey</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Greg</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Arielie</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Lisa</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Bob</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>5</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>John</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Joey</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Greg</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Arielie</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Lisa</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Bob</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>6</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>John</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Joey</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Greg</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Arielie</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Lisa</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Bob</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>